<commit_message>
feat: Add Excel export functionality to Batch and Course pages, enhance data formatting and UI components
</commit_message>
<xml_diff>
--- a/src/assets/Course_Template-Instruction.xlsx
+++ b/src/assets/Course_Template-Instruction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="8250" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="TemplateCourse Template" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>Sl No</t>
   </si>
@@ -23,24 +23,18 @@
     <t>Course Name</t>
   </si>
   <si>
+    <t>QPNOS Code</t>
+  </si>
+  <si>
     <t>From Date</t>
   </si>
   <si>
     <t>To Date</t>
   </si>
   <si>
-    <t>Theory Duration Hours</t>
-  </si>
-  <si>
-    <t>Practical Duration Hours</t>
-  </si>
-  <si>
     <t>Sector Name</t>
   </si>
   <si>
-    <t>Course Code</t>
-  </si>
-  <si>
     <t>Field Name</t>
   </si>
   <si>
@@ -68,7 +62,7 @@
     <t>1, 2, 3, ...</t>
   </si>
   <si>
-    <t>Job Role Name</t>
+    <t>Course Name (Job Role Name)</t>
   </si>
   <si>
     <t>String</t>
@@ -92,28 +86,16 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Start date of the course (YYYY-MM-DD format)</t>
-  </si>
-  <si>
-    <t>"2024-04-01"</t>
-  </si>
-  <si>
-    <t>End date of the course (YYYY-MM-DD format)</t>
-  </si>
-  <si>
-    <t>"2024-06-30"</t>
-  </si>
-  <si>
-    <t>Total hours allocated for theory sessions</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>Total hours allocated for practical sessions</t>
-  </si>
-  <si>
-    <t>200</t>
+    <t>Start date of the course (YYYY/MM/DD format)</t>
+  </si>
+  <si>
+    <t>"2024/04/01"</t>
+  </si>
+  <si>
+    <t>End date of the course (YYYY/MM/DD format)</t>
+  </si>
+  <si>
+    <t>"2024/06/30"</t>
   </si>
   <si>
     <t>String (Dropdown)</t>
@@ -257,18 +239,14 @@
     </r>
   </si>
   <si>
-    <t>3. Use an already registered sector on ASDM or add your own sector from the Convergence Portal. To do so, first add the sector in the portal before using it.</t>
+    <t>3. The QP/NOS Code is linked with other fields, and any mismatch in the associated data may result in an error."</t>
+  </si>
+  <si>
+    <t>4. Use an already registered sector on ASDM or add your own sector from the Convergence Portal. To do so, first add the sector in the portal before using it.</t>
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4.</t>
+      <t>5.</t>
     </r>
     <r>
       <rPr>
@@ -298,12 +276,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -330,13 +308,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -357,25 +328,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -388,7 +344,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -410,55 +366,49 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -471,6 +421,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -478,6 +442,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -486,7 +457,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -501,25 +472,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -531,157 +646,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,21 +681,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -739,6 +695,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -758,17 +729,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -780,15 +740,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -807,165 +758,184 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1351,24 +1321,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showFormulas="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="$A2:$XFD2 $A3:$XFD3"/>
+    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
     <col min="2" max="2" width="13.7533333333333" customWidth="1"/>
-    <col min="3" max="3" width="10.2533333333333" customWidth="1"/>
-    <col min="4" max="4" width="8.25333333333333" customWidth="1"/>
-    <col min="5" max="5" width="19.6666666666667" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="16.08" customWidth="1"/>
-    <col min="8" max="8" width="14.08" customWidth="1"/>
+    <col min="3" max="3" width="8.2" customWidth="1"/>
+    <col min="4" max="4" width="10.2533333333333" customWidth="1"/>
+    <col min="5" max="5" width="8.25333333333333" customWidth="1"/>
+    <col min="6" max="6" width="16.08" customWidth="1"/>
+    <col min="7" max="7" width="14.08" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1387,43 +1356,24 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="3:4">
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="3:7">
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="6" spans="8:8">
-      <c r="H6" s="7"/>
+    </row>
+    <row r="2" spans="4:5">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="4:6">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="6" spans="7:7">
+      <c r="G6" s="6"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="whole" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Number" prompt="Only Accept Numbers" sqref="F2:F1048576">
-      <formula1>0</formula1>
-      <formula2>9999999999</formula2>
-    </dataValidation>
-    <dataValidation type="whole" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
-      <formula1>0</formula1>
-      <formula2>9999999999</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Number" prompt="Only Accept Numbers" sqref="F1"/>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="G1 A1:D1" numberStoredAsText="1"/>
+    <ignoredError sqref="D1:E1 A1:B1 F1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1431,34 +1381,36 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.5" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="3" width="35.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="52.8" style="1" customWidth="1"/>
     <col min="5" max="16384" width="35.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:5">
@@ -1466,160 +1418,131 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:5">
       <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:5">
       <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="1" t="s">
+    </row>
+    <row r="10" s="1" customFormat="1" spans="1:1">
+      <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" s="1" customFormat="1" spans="1:5">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1" t="s">
+    <row r="11" s="1" customFormat="1" ht="27" customHeight="1" spans="1:1">
+      <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="1" t="s">
+    </row>
+    <row r="12" s="1" customFormat="1" ht="27" customHeight="1" spans="1:1">
+      <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" s="1" customFormat="1" spans="1:5">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1" t="s">
+    <row r="13" s="1" customFormat="1" ht="27" customHeight="1" spans="1:1">
+      <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="1" t="s">
+    </row>
+    <row r="14" s="1" customFormat="1" ht="27" customHeight="1" spans="1:1">
+      <c r="A14" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" s="1" customFormat="1" spans="1:1">
-      <c r="A12" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" s="1" customFormat="1" ht="27" customHeight="1" spans="1:1">
-      <c r="A13" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" s="1" customFormat="1" ht="27" customHeight="1" spans="1:1">
-      <c r="A14" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="1" ht="27" customHeight="1" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" s="1" customFormat="1" ht="27" customHeight="1" spans="1:1">
-      <c r="A16" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>